<commit_message>
update some torch output files
</commit_message>
<xml_diff>
--- a/outputs/torch/alexnet.xlsx
+++ b/outputs/torch/alexnet.xlsx
@@ -123,7 +123,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -142,13 +142,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="0000FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="00FFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -514,7 +507,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
@@ -539,57 +532,58 @@
       <c r="E1" s="12" t="n"/>
       <c r="F1" s="10" t="inlineStr">
         <is>
+          <t>Connection</t>
+        </is>
+      </c>
+      <c r="G1" s="11" t="n"/>
+      <c r="H1" s="11" t="n"/>
+      <c r="I1" s="12" t="n"/>
+      <c r="J1" s="10" t="inlineStr">
+        <is>
           <t>Input Dimension</t>
         </is>
       </c>
-      <c r="G1" s="11" t="n"/>
-      <c r="H1" s="12" t="n"/>
-      <c r="I1" s="10" t="inlineStr">
+      <c r="K1" s="11" t="n"/>
+      <c r="L1" s="12" t="n"/>
+      <c r="M1" s="10" t="inlineStr">
         <is>
           <t>Output Dimension</t>
         </is>
       </c>
-      <c r="J1" s="11" t="n"/>
-      <c r="K1" s="12" t="n"/>
-      <c r="L1" s="10" t="inlineStr">
-        <is>
-          <t>Kernel</t>
-        </is>
-      </c>
-      <c r="M1" s="12" t="n"/>
-      <c r="N1" s="10" t="inlineStr">
-        <is>
-          <t>Stride</t>
-        </is>
-      </c>
+      <c r="N1" s="11" t="n"/>
       <c r="O1" s="12" t="n"/>
       <c r="P1" s="10" t="inlineStr">
         <is>
-          <t>Padding</t>
+          <t>Kernel</t>
         </is>
       </c>
       <c r="Q1" s="12" t="n"/>
       <c r="R1" s="10" t="inlineStr">
         <is>
+          <t>Stride</t>
+        </is>
+      </c>
+      <c r="S1" s="12" t="n"/>
+      <c r="T1" s="10" t="inlineStr">
+        <is>
+          <t>Padding</t>
+        </is>
+      </c>
+      <c r="U1" s="12" t="n"/>
+      <c r="V1" s="10" t="inlineStr">
+        <is>
           <t>Size of Parameters</t>
         </is>
       </c>
-      <c r="S1" s="11" t="n"/>
-      <c r="T1" s="12" t="n"/>
-      <c r="U1" s="10" t="inlineStr">
+      <c r="W1" s="11" t="n"/>
+      <c r="X1" s="12" t="n"/>
+      <c r="Y1" s="10" t="inlineStr">
         <is>
           <t>Forward Ops</t>
         </is>
       </c>
-      <c r="V1" s="11" t="n"/>
-      <c r="W1" s="12" t="n"/>
-      <c r="X1" s="10" t="inlineStr">
-        <is>
-          <t>Backward Ops</t>
-        </is>
-      </c>
-      <c r="Y1" s="11" t="n"/>
-      <c r="Z1" s="12" t="n"/>
+      <c r="Z1" s="11" t="n"/>
+      <c r="AA1" s="12" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="10" t="inlineStr"/>
@@ -615,105 +609,110 @@
       </c>
       <c r="F2" s="10" t="inlineStr">
         <is>
+          <t>input0</t>
+        </is>
+      </c>
+      <c r="G2" s="10" t="inlineStr">
+        <is>
+          <t>input1</t>
+        </is>
+      </c>
+      <c r="H2" s="10" t="inlineStr">
+        <is>
+          <t>output0</t>
+        </is>
+      </c>
+      <c r="I2" s="10" t="inlineStr">
+        <is>
+          <t>output1</t>
+        </is>
+      </c>
+      <c r="J2" s="10" t="inlineStr">
+        <is>
           <t>Channel</t>
         </is>
       </c>
-      <c r="G2" s="10" t="inlineStr">
+      <c r="K2" s="10" t="inlineStr">
         <is>
           <t>Height</t>
         </is>
       </c>
-      <c r="H2" s="10" t="inlineStr">
+      <c r="L2" s="10" t="inlineStr">
         <is>
           <t>Width</t>
         </is>
       </c>
-      <c r="I2" s="10" t="inlineStr">
+      <c r="M2" s="10" t="inlineStr">
         <is>
           <t>Channel</t>
         </is>
       </c>
-      <c r="J2" s="10" t="inlineStr">
+      <c r="N2" s="10" t="inlineStr">
         <is>
           <t>Height</t>
         </is>
       </c>
-      <c r="K2" s="10" t="inlineStr">
+      <c r="O2" s="10" t="inlineStr">
         <is>
           <t>Width</t>
         </is>
       </c>
-      <c r="L2" s="10" t="inlineStr">
+      <c r="P2" s="10" t="inlineStr">
         <is>
           <t>Height</t>
         </is>
       </c>
-      <c r="M2" s="10" t="inlineStr">
+      <c r="Q2" s="10" t="inlineStr">
         <is>
           <t>Width</t>
         </is>
       </c>
-      <c r="N2" s="10" t="inlineStr">
+      <c r="R2" s="10" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="O2" s="10" t="inlineStr">
+      <c r="S2" s="10" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="P2" s="10" t="inlineStr">
+      <c r="T2" s="10" t="inlineStr">
         <is>
           <t>X</t>
         </is>
       </c>
-      <c r="Q2" s="10" t="inlineStr">
+      <c r="U2" s="10" t="inlineStr">
         <is>
           <t>Y</t>
         </is>
       </c>
-      <c r="R2" s="10" t="inlineStr">
+      <c r="V2" s="10" t="inlineStr">
         <is>
           <t>Input</t>
         </is>
       </c>
-      <c r="S2" s="10" t="inlineStr">
+      <c r="W2" s="10" t="inlineStr">
         <is>
           <t>Output</t>
         </is>
       </c>
-      <c r="T2" s="10" t="inlineStr">
+      <c r="X2" s="10" t="inlineStr">
         <is>
           <t>Weight</t>
         </is>
       </c>
-      <c r="U2" s="10" t="inlineStr">
+      <c r="Y2" s="10" t="inlineStr">
         <is>
           <t>GEMM</t>
         </is>
       </c>
-      <c r="V2" s="10" t="inlineStr">
+      <c r="Z2" s="10" t="inlineStr">
         <is>
           <t>ElemWise</t>
         </is>
       </c>
-      <c r="W2" s="10" t="inlineStr">
-        <is>
-          <t>Activation</t>
-        </is>
-      </c>
-      <c r="X2" s="10" t="inlineStr">
-        <is>
-          <t>GEMM</t>
-        </is>
-      </c>
-      <c r="Y2" s="10" t="inlineStr">
-        <is>
-          <t>ElemWise</t>
-        </is>
-      </c>
-      <c r="Z2" s="10" t="inlineStr">
+      <c r="AA2" s="10" t="inlineStr">
         <is>
           <t>Activation</t>
         </is>
@@ -731,43 +730,52 @@
       <c r="C3" s="8" t="n"/>
       <c r="D3" s="8" t="n"/>
       <c r="E3" s="8" t="n"/>
-      <c r="F3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="8" t="n">
-        <v>0</v>
-      </c>
+      <c r="F3" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-12</t>
+        </is>
+      </c>
+      <c r="G3" s="8" t="n"/>
+      <c r="H3" s="8" t="inlineStr">
+        <is>
+          <t>AdaptiveAvgPool2d: 1-2</t>
+        </is>
+      </c>
+      <c r="I3" s="8" t="n"/>
       <c r="J3" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K3" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="L3" s="8" t="n"/>
-      <c r="M3" s="8" t="n"/>
-      <c r="N3" s="8" t="n"/>
-      <c r="O3" s="8" t="n"/>
+      <c r="L3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="8" t="n">
+        <v>0</v>
+      </c>
       <c r="P3" s="8" t="n"/>
       <c r="Q3" s="8" t="n"/>
-      <c r="R3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S3" s="8" t="n">
-        <v>0</v>
-      </c>
+      <c r="R3" s="8" t="n"/>
+      <c r="S3" s="8" t="n"/>
       <c r="T3" s="8" t="n"/>
       <c r="U3" s="8" t="n"/>
-      <c r="V3" s="8" t="n"/>
-      <c r="W3" s="8" t="n"/>
+      <c r="V3" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="8" t="n">
+        <v>0</v>
+      </c>
       <c r="X3" s="8" t="n"/>
       <c r="Y3" s="8" t="n"/>
       <c r="Z3" s="8" t="n"/>
+      <c r="AA3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="7" t="n">
@@ -781,61 +789,64 @@
       </c>
       <c r="D4" s="8" t="n"/>
       <c r="E4" s="8" t="n"/>
-      <c r="F4" s="8" t="n">
+      <c r="F4" s="8" t="n"/>
+      <c r="G4" s="8" t="n"/>
+      <c r="H4" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-2</t>
+        </is>
+      </c>
+      <c r="I4" s="8" t="n"/>
+      <c r="J4" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="8" t="n">
+      <c r="K4" s="8" t="n">
         <v>224</v>
       </c>
-      <c r="H4" s="8" t="n">
+      <c r="L4" s="8" t="n">
         <v>224</v>
       </c>
-      <c r="I4" s="8" t="n">
+      <c r="M4" s="8" t="n">
         <v>64</v>
       </c>
-      <c r="J4" s="8" t="n">
+      <c r="N4" s="8" t="n">
         <v>55</v>
       </c>
-      <c r="K4" s="8" t="n">
+      <c r="O4" s="8" t="n">
         <v>55</v>
       </c>
-      <c r="L4" s="8" t="n">
+      <c r="P4" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="M4" s="8" t="n">
+      <c r="Q4" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="N4" s="8" t="n">
+      <c r="R4" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="O4" s="8" t="n">
+      <c r="S4" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="P4" s="8" t="n">
+      <c r="T4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="Q4" s="8" t="n">
+      <c r="U4" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="R4" s="8" t="n">
+      <c r="V4" s="8" t="n">
         <v>150528</v>
       </c>
-      <c r="S4" s="8" t="n">
+      <c r="W4" s="8" t="n">
         <v>193600</v>
       </c>
-      <c r="T4" s="8" t="n">
+      <c r="X4" s="8" t="n">
         <v>23296</v>
       </c>
-      <c r="U4" s="8" t="n">
+      <c r="Y4" s="8" t="n">
         <v>70470400</v>
       </c>
-      <c r="V4" s="8" t="n"/>
-      <c r="W4" s="8" t="n"/>
-      <c r="X4" s="8" t="n">
-        <v>1165688832</v>
-      </c>
-      <c r="Y4" s="8" t="n"/>
       <c r="Z4" s="8" t="n"/>
+      <c r="AA4" s="8" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="7" t="n">
@@ -844,50 +855,57 @@
       <c r="B5" s="8" t="n"/>
       <c r="C5" s="8" t="inlineStr">
         <is>
-          <t>ReLU: 2-2</t>
+          <t>ReLU(inplace): 2-2</t>
         </is>
       </c>
       <c r="D5" s="8" t="n"/>
       <c r="E5" s="8" t="n"/>
-      <c r="F5" s="8" t="n">
+      <c r="F5" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-1</t>
+        </is>
+      </c>
+      <c r="G5" s="8" t="n"/>
+      <c r="H5" s="8" t="inlineStr">
+        <is>
+          <t>MaxPool2d: 2-3</t>
+        </is>
+      </c>
+      <c r="I5" s="8" t="n"/>
+      <c r="J5" s="8" t="n">
         <v>64</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>55</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>55</v>
-      </c>
-      <c r="I5" s="8" t="n">
-        <v>64</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>55</v>
       </c>
       <c r="K5" s="8" t="n">
         <v>55</v>
       </c>
-      <c r="L5" s="8" t="n"/>
-      <c r="M5" s="8" t="n"/>
-      <c r="N5" s="8" t="n"/>
-      <c r="O5" s="8" t="n"/>
+      <c r="L5" s="8" t="n">
+        <v>55</v>
+      </c>
+      <c r="M5" s="8" t="n">
+        <v>64</v>
+      </c>
+      <c r="N5" s="8" t="n">
+        <v>55</v>
+      </c>
+      <c r="O5" s="8" t="n">
+        <v>55</v>
+      </c>
       <c r="P5" s="8" t="n"/>
       <c r="Q5" s="8" t="n"/>
-      <c r="R5" s="8" t="n">
-        <v>193600</v>
-      </c>
-      <c r="S5" s="8" t="n">
-        <v>193600</v>
-      </c>
+      <c r="R5" s="8" t="n"/>
+      <c r="S5" s="8" t="n"/>
       <c r="T5" s="8" t="n"/>
       <c r="U5" s="8" t="n"/>
-      <c r="V5" s="8" t="n"/>
+      <c r="V5" s="8" t="n">
+        <v>193600</v>
+      </c>
       <c r="W5" s="8" t="n">
         <v>193600</v>
       </c>
       <c r="X5" s="8" t="n"/>
       <c r="Y5" s="8" t="n"/>
-      <c r="Z5" s="8" t="n">
+      <c r="Z5" s="8" t="n"/>
+      <c r="AA5" s="8" t="n">
         <v>193600</v>
       </c>
     </row>
@@ -903,55 +921,62 @@
       </c>
       <c r="D6" s="8" t="n"/>
       <c r="E6" s="8" t="n"/>
-      <c r="F6" s="8" t="n">
+      <c r="F6" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-2</t>
+        </is>
+      </c>
+      <c r="G6" s="8" t="n"/>
+      <c r="H6" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-4</t>
+        </is>
+      </c>
+      <c r="I6" s="8" t="n"/>
+      <c r="J6" s="8" t="n">
         <v>64</v>
       </c>
-      <c r="G6" s="8" t="n">
+      <c r="K6" s="8" t="n">
         <v>55</v>
       </c>
-      <c r="H6" s="8" t="n">
+      <c r="L6" s="8" t="n">
         <v>55</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="M6" s="8" t="n">
         <v>64</v>
       </c>
-      <c r="J6" s="8" t="n">
+      <c r="N6" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="K6" s="8" t="n">
+      <c r="O6" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="L6" s="8" t="n">
+      <c r="P6" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="M6" s="8" t="n">
+      <c r="Q6" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N6" s="8" t="n">
+      <c r="R6" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="O6" s="8" t="n"/>
-      <c r="P6" s="8" t="n">
+      <c r="S6" s="8" t="n"/>
+      <c r="T6" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="Q6" s="8" t="n"/>
-      <c r="R6" s="8" t="n">
-        <v>193600</v>
-      </c>
-      <c r="S6" s="8" t="n">
-        <v>46656</v>
-      </c>
-      <c r="T6" s="8" t="n"/>
       <c r="U6" s="8" t="n"/>
       <c r="V6" s="8" t="n">
+        <v>193600</v>
+      </c>
+      <c r="W6" s="8" t="n">
+        <v>46656</v>
+      </c>
+      <c r="X6" s="8" t="n"/>
+      <c r="Y6" s="8" t="n"/>
+      <c r="Z6" s="8" t="n">
         <v>373248</v>
       </c>
-      <c r="W6" s="8" t="n"/>
-      <c r="X6" s="8" t="n"/>
-      <c r="Y6" s="8" t="n">
-        <v>141134400</v>
-      </c>
-      <c r="Z6" s="8" t="n"/>
+      <c r="AA6" s="8" t="n"/>
     </row>
     <row r="7">
       <c r="A7" s="7" t="n">
@@ -965,61 +990,68 @@
       </c>
       <c r="D7" s="8" t="n"/>
       <c r="E7" s="8" t="n"/>
-      <c r="F7" s="8" t="n">
+      <c r="F7" s="8" t="inlineStr">
+        <is>
+          <t>MaxPool2d: 2-3</t>
+        </is>
+      </c>
+      <c r="G7" s="8" t="n"/>
+      <c r="H7" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-5</t>
+        </is>
+      </c>
+      <c r="I7" s="8" t="n"/>
+      <c r="J7" s="8" t="n">
         <v>64</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>27</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>27</v>
-      </c>
-      <c r="I7" s="8" t="n">
-        <v>192</v>
-      </c>
-      <c r="J7" s="8" t="n">
-        <v>27</v>
       </c>
       <c r="K7" s="8" t="n">
         <v>27</v>
       </c>
       <c r="L7" s="8" t="n">
+        <v>27</v>
+      </c>
+      <c r="M7" s="8" t="n">
+        <v>192</v>
+      </c>
+      <c r="N7" s="8" t="n">
+        <v>27</v>
+      </c>
+      <c r="O7" s="8" t="n">
+        <v>27</v>
+      </c>
+      <c r="P7" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="M7" s="8" t="n">
+      <c r="Q7" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="N7" s="8" t="n">
+      <c r="R7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="8" t="n">
+      <c r="S7" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P7" s="8" t="n">
+      <c r="T7" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="Q7" s="8" t="n">
+      <c r="U7" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="R7" s="8" t="n">
+      <c r="V7" s="8" t="n">
         <v>46656</v>
       </c>
-      <c r="S7" s="8" t="n">
+      <c r="W7" s="8" t="n">
         <v>139968</v>
       </c>
-      <c r="T7" s="8" t="n">
+      <c r="X7" s="8" t="n">
         <v>307392</v>
       </c>
-      <c r="U7" s="8" t="n">
+      <c r="Y7" s="8" t="n">
         <v>224088768</v>
       </c>
-      <c r="V7" s="8" t="n"/>
-      <c r="W7" s="8" t="n"/>
-      <c r="X7" s="8" t="n">
-        <v>223948800</v>
-      </c>
-      <c r="Y7" s="8" t="n"/>
       <c r="Z7" s="8" t="n"/>
+      <c r="AA7" s="8" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="7" t="n">
@@ -1028,50 +1060,57 @@
       <c r="B8" s="8" t="n"/>
       <c r="C8" s="8" t="inlineStr">
         <is>
-          <t>ReLU: 2-5</t>
+          <t>ReLU(inplace): 2-5</t>
         </is>
       </c>
       <c r="D8" s="8" t="n"/>
       <c r="E8" s="8" t="n"/>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-4</t>
+        </is>
+      </c>
+      <c r="G8" s="8" t="n"/>
+      <c r="H8" s="8" t="inlineStr">
+        <is>
+          <t>MaxPool2d: 2-6</t>
+        </is>
+      </c>
+      <c r="I8" s="8" t="n"/>
+      <c r="J8" s="8" t="n">
         <v>192</v>
-      </c>
-      <c r="G8" s="8" t="n">
-        <v>27</v>
-      </c>
-      <c r="H8" s="8" t="n">
-        <v>27</v>
-      </c>
-      <c r="I8" s="8" t="n">
-        <v>192</v>
-      </c>
-      <c r="J8" s="8" t="n">
-        <v>27</v>
       </c>
       <c r="K8" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="L8" s="8" t="n"/>
-      <c r="M8" s="8" t="n"/>
-      <c r="N8" s="8" t="n"/>
-      <c r="O8" s="8" t="n"/>
+      <c r="L8" s="8" t="n">
+        <v>27</v>
+      </c>
+      <c r="M8" s="8" t="n">
+        <v>192</v>
+      </c>
+      <c r="N8" s="8" t="n">
+        <v>27</v>
+      </c>
+      <c r="O8" s="8" t="n">
+        <v>27</v>
+      </c>
       <c r="P8" s="8" t="n"/>
       <c r="Q8" s="8" t="n"/>
-      <c r="R8" s="8" t="n">
-        <v>139968</v>
-      </c>
-      <c r="S8" s="8" t="n">
-        <v>139968</v>
-      </c>
+      <c r="R8" s="8" t="n"/>
+      <c r="S8" s="8" t="n"/>
       <c r="T8" s="8" t="n"/>
       <c r="U8" s="8" t="n"/>
-      <c r="V8" s="8" t="n"/>
+      <c r="V8" s="8" t="n">
+        <v>139968</v>
+      </c>
       <c r="W8" s="8" t="n">
         <v>139968</v>
       </c>
       <c r="X8" s="8" t="n"/>
       <c r="Y8" s="8" t="n"/>
-      <c r="Z8" s="8" t="n">
+      <c r="Z8" s="8" t="n"/>
+      <c r="AA8" s="8" t="n">
         <v>139968</v>
       </c>
     </row>
@@ -1087,55 +1126,62 @@
       </c>
       <c r="D9" s="8" t="n"/>
       <c r="E9" s="8" t="n"/>
-      <c r="F9" s="8" t="n">
+      <c r="F9" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-5</t>
+        </is>
+      </c>
+      <c r="G9" s="8" t="n"/>
+      <c r="H9" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-7</t>
+        </is>
+      </c>
+      <c r="I9" s="8" t="n"/>
+      <c r="J9" s="8" t="n">
         <v>192</v>
       </c>
-      <c r="G9" s="8" t="n">
+      <c r="K9" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="L9" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="M9" s="8" t="n">
         <v>192</v>
       </c>
-      <c r="J9" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="K9" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="L9" s="8" t="n">
+      <c r="N9" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="O9" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="P9" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="M9" s="8" t="n">
+      <c r="Q9" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N9" s="8" t="n">
+      <c r="R9" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="O9" s="8" t="n"/>
-      <c r="P9" s="8" t="n">
+      <c r="S9" s="8" t="n"/>
+      <c r="T9" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="Q9" s="8" t="n"/>
-      <c r="R9" s="8" t="n">
-        <v>139968</v>
-      </c>
-      <c r="S9" s="8" t="n">
-        <v>32448</v>
-      </c>
-      <c r="T9" s="8" t="n"/>
       <c r="U9" s="8" t="n"/>
       <c r="V9" s="8" t="n">
+        <v>139968</v>
+      </c>
+      <c r="W9" s="8" t="n">
+        <v>32448</v>
+      </c>
+      <c r="X9" s="8" t="n"/>
+      <c r="Y9" s="8" t="n"/>
+      <c r="Z9" s="8" t="n">
         <v>259584</v>
       </c>
-      <c r="W9" s="8" t="n"/>
-      <c r="X9" s="8" t="n"/>
-      <c r="Y9" s="8" t="n">
-        <v>23654592</v>
-      </c>
-      <c r="Z9" s="8" t="n"/>
+      <c r="AA9" s="8" t="n"/>
     </row>
     <row r="10">
       <c r="A10" s="7" t="n">
@@ -1149,61 +1195,68 @@
       </c>
       <c r="D10" s="8" t="n"/>
       <c r="E10" s="8" t="n"/>
-      <c r="F10" s="8" t="n">
+      <c r="F10" s="8" t="inlineStr">
+        <is>
+          <t>MaxPool2d: 2-6</t>
+        </is>
+      </c>
+      <c r="G10" s="8" t="n"/>
+      <c r="H10" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-8</t>
+        </is>
+      </c>
+      <c r="I10" s="8" t="n"/>
+      <c r="J10" s="8" t="n">
         <v>192</v>
       </c>
-      <c r="G10" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="H10" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="I10" s="8" t="n">
+      <c r="K10" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L10" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="M10" s="8" t="n">
         <v>384</v>
       </c>
-      <c r="J10" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="K10" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="L10" s="8" t="n">
+      <c r="N10" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="O10" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="P10" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="M10" s="8" t="n">
+      <c r="Q10" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N10" s="8" t="n">
+      <c r="R10" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="O10" s="8" t="n">
+      <c r="S10" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P10" s="8" t="n">
+      <c r="T10" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="Q10" s="8" t="n">
+      <c r="U10" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="R10" s="8" t="n">
+      <c r="V10" s="8" t="n">
         <v>32448</v>
       </c>
-      <c r="S10" s="8" t="n">
+      <c r="W10" s="8" t="n">
         <v>64896</v>
       </c>
-      <c r="T10" s="8" t="n">
+      <c r="X10" s="8" t="n">
         <v>663936</v>
       </c>
-      <c r="U10" s="8" t="n">
+      <c r="Y10" s="8" t="n">
         <v>112205184</v>
       </c>
-      <c r="V10" s="8" t="n"/>
-      <c r="W10" s="8" t="n"/>
-      <c r="X10" s="8" t="n">
-        <v>112140288</v>
-      </c>
-      <c r="Y10" s="8" t="n"/>
       <c r="Z10" s="8" t="n"/>
+      <c r="AA10" s="8" t="n"/>
     </row>
     <row r="11">
       <c r="A11" s="7" t="n">
@@ -1212,50 +1265,57 @@
       <c r="B11" s="8" t="n"/>
       <c r="C11" s="8" t="inlineStr">
         <is>
-          <t>ReLU: 2-8</t>
+          <t>ReLU(inplace): 2-8</t>
         </is>
       </c>
       <c r="D11" s="8" t="n"/>
       <c r="E11" s="8" t="n"/>
-      <c r="F11" s="8" t="n">
+      <c r="F11" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-7</t>
+        </is>
+      </c>
+      <c r="G11" s="8" t="n"/>
+      <c r="H11" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-9</t>
+        </is>
+      </c>
+      <c r="I11" s="8" t="n"/>
+      <c r="J11" s="8" t="n">
         <v>384</v>
       </c>
-      <c r="G11" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="H11" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="I11" s="8" t="n">
+      <c r="K11" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L11" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="M11" s="8" t="n">
         <v>384</v>
       </c>
-      <c r="J11" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="K11" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="L11" s="8" t="n"/>
-      <c r="M11" s="8" t="n"/>
-      <c r="N11" s="8" t="n"/>
-      <c r="O11" s="8" t="n"/>
+      <c r="N11" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="O11" s="8" t="n">
+        <v>13</v>
+      </c>
       <c r="P11" s="8" t="n"/>
       <c r="Q11" s="8" t="n"/>
-      <c r="R11" s="8" t="n">
-        <v>64896</v>
-      </c>
-      <c r="S11" s="8" t="n">
-        <v>64896</v>
-      </c>
+      <c r="R11" s="8" t="n"/>
+      <c r="S11" s="8" t="n"/>
       <c r="T11" s="8" t="n"/>
       <c r="U11" s="8" t="n"/>
-      <c r="V11" s="8" t="n"/>
+      <c r="V11" s="8" t="n">
+        <v>64896</v>
+      </c>
       <c r="W11" s="8" t="n">
         <v>64896</v>
       </c>
       <c r="X11" s="8" t="n"/>
       <c r="Y11" s="8" t="n"/>
-      <c r="Z11" s="8" t="n">
+      <c r="Z11" s="8" t="n"/>
+      <c r="AA11" s="8" t="n">
         <v>64896</v>
       </c>
     </row>
@@ -1271,61 +1331,68 @@
       </c>
       <c r="D12" s="8" t="n"/>
       <c r="E12" s="8" t="n"/>
-      <c r="F12" s="8" t="n">
+      <c r="F12" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-8</t>
+        </is>
+      </c>
+      <c r="G12" s="8" t="n"/>
+      <c r="H12" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-10</t>
+        </is>
+      </c>
+      <c r="I12" s="8" t="n"/>
+      <c r="J12" s="8" t="n">
         <v>384</v>
       </c>
-      <c r="G12" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="H12" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="I12" s="8" t="n">
+      <c r="K12" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L12" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="M12" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="J12" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="K12" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="L12" s="8" t="n">
+      <c r="N12" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="O12" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="P12" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="M12" s="8" t="n">
+      <c r="Q12" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N12" s="8" t="n">
+      <c r="R12" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="O12" s="8" t="n">
+      <c r="S12" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P12" s="8" t="n">
+      <c r="T12" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="Q12" s="8" t="n">
+      <c r="U12" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="R12" s="8" t="n">
+      <c r="V12" s="8" t="n">
         <v>64896</v>
       </c>
-      <c r="S12" s="8" t="n">
+      <c r="W12" s="8" t="n">
         <v>43264</v>
       </c>
-      <c r="T12" s="8" t="n">
+      <c r="X12" s="8" t="n">
         <v>884992</v>
       </c>
-      <c r="U12" s="8" t="n">
+      <c r="Y12" s="8" t="n">
         <v>149563648</v>
       </c>
-      <c r="V12" s="8" t="n"/>
-      <c r="W12" s="8" t="n"/>
-      <c r="X12" s="8" t="n">
-        <v>149520384</v>
-      </c>
-      <c r="Y12" s="8" t="n"/>
       <c r="Z12" s="8" t="n"/>
+      <c r="AA12" s="8" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="7" t="n">
@@ -1334,50 +1401,57 @@
       <c r="B13" s="8" t="n"/>
       <c r="C13" s="8" t="inlineStr">
         <is>
-          <t>ReLU: 2-10</t>
+          <t>ReLU(inplace): 2-10</t>
         </is>
       </c>
       <c r="D13" s="8" t="n"/>
       <c r="E13" s="8" t="n"/>
-      <c r="F13" s="8" t="n">
+      <c r="F13" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-9</t>
+        </is>
+      </c>
+      <c r="G13" s="8" t="n"/>
+      <c r="H13" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-11</t>
+        </is>
+      </c>
+      <c r="I13" s="8" t="n"/>
+      <c r="J13" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="G13" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="H13" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="I13" s="8" t="n">
+      <c r="K13" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L13" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="M13" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="J13" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="K13" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="L13" s="8" t="n"/>
-      <c r="M13" s="8" t="n"/>
-      <c r="N13" s="8" t="n"/>
-      <c r="O13" s="8" t="n"/>
+      <c r="N13" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="O13" s="8" t="n">
+        <v>13</v>
+      </c>
       <c r="P13" s="8" t="n"/>
       <c r="Q13" s="8" t="n"/>
-      <c r="R13" s="8" t="n">
-        <v>43264</v>
-      </c>
-      <c r="S13" s="8" t="n">
-        <v>43264</v>
-      </c>
+      <c r="R13" s="8" t="n"/>
+      <c r="S13" s="8" t="n"/>
       <c r="T13" s="8" t="n"/>
       <c r="U13" s="8" t="n"/>
-      <c r="V13" s="8" t="n"/>
+      <c r="V13" s="8" t="n">
+        <v>43264</v>
+      </c>
       <c r="W13" s="8" t="n">
         <v>43264</v>
       </c>
       <c r="X13" s="8" t="n"/>
       <c r="Y13" s="8" t="n"/>
-      <c r="Z13" s="8" t="n">
+      <c r="Z13" s="8" t="n"/>
+      <c r="AA13" s="8" t="n">
         <v>43264</v>
       </c>
     </row>
@@ -1393,61 +1467,68 @@
       </c>
       <c r="D14" s="8" t="n"/>
       <c r="E14" s="8" t="n"/>
-      <c r="F14" s="8" t="n">
+      <c r="F14" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-10</t>
+        </is>
+      </c>
+      <c r="G14" s="8" t="n"/>
+      <c r="H14" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-12</t>
+        </is>
+      </c>
+      <c r="I14" s="8" t="n"/>
+      <c r="J14" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="G14" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="H14" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="I14" s="8" t="n">
+      <c r="K14" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L14" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="M14" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="J14" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="K14" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="L14" s="8" t="n">
+      <c r="N14" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="O14" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="P14" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="M14" s="8" t="n">
+      <c r="Q14" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N14" s="8" t="n">
+      <c r="R14" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="O14" s="8" t="n">
+      <c r="S14" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="P14" s="8" t="n">
+      <c r="T14" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="Q14" s="8" t="n">
+      <c r="U14" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="R14" s="8" t="n">
+      <c r="V14" s="8" t="n">
         <v>43264</v>
       </c>
-      <c r="S14" s="8" t="n">
+      <c r="W14" s="8" t="n">
         <v>43264</v>
       </c>
-      <c r="T14" s="8" t="n">
+      <c r="X14" s="8" t="n">
         <v>590080</v>
       </c>
-      <c r="U14" s="8" t="n">
+      <c r="Y14" s="8" t="n">
         <v>99723520</v>
       </c>
-      <c r="V14" s="8" t="n"/>
-      <c r="W14" s="8" t="n"/>
-      <c r="X14" s="8" t="n">
-        <v>99680256</v>
-      </c>
-      <c r="Y14" s="8" t="n"/>
       <c r="Z14" s="8" t="n"/>
+      <c r="AA14" s="8" t="n"/>
     </row>
     <row r="15">
       <c r="A15" s="7" t="n">
@@ -1456,50 +1537,57 @@
       <c r="B15" s="8" t="n"/>
       <c r="C15" s="8" t="inlineStr">
         <is>
-          <t>ReLU: 2-12</t>
+          <t>ReLU(inplace): 2-12</t>
         </is>
       </c>
       <c r="D15" s="8" t="n"/>
       <c r="E15" s="8" t="n"/>
-      <c r="F15" s="8" t="n">
+      <c r="F15" s="8" t="inlineStr">
+        <is>
+          <t>Conv2d: 2-11</t>
+        </is>
+      </c>
+      <c r="G15" s="8" t="n"/>
+      <c r="H15" s="8" t="inlineStr">
+        <is>
+          <t>MaxPool2d: 2-13</t>
+        </is>
+      </c>
+      <c r="I15" s="8" t="n"/>
+      <c r="J15" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="G15" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="H15" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="I15" s="8" t="n">
+      <c r="K15" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L15" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="M15" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="J15" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="K15" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="L15" s="8" t="n"/>
-      <c r="M15" s="8" t="n"/>
-      <c r="N15" s="8" t="n"/>
-      <c r="O15" s="8" t="n"/>
+      <c r="N15" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="O15" s="8" t="n">
+        <v>13</v>
+      </c>
       <c r="P15" s="8" t="n"/>
       <c r="Q15" s="8" t="n"/>
-      <c r="R15" s="8" t="n">
-        <v>43264</v>
-      </c>
-      <c r="S15" s="8" t="n">
-        <v>43264</v>
-      </c>
+      <c r="R15" s="8" t="n"/>
+      <c r="S15" s="8" t="n"/>
       <c r="T15" s="8" t="n"/>
       <c r="U15" s="8" t="n"/>
-      <c r="V15" s="8" t="n"/>
+      <c r="V15" s="8" t="n">
+        <v>43264</v>
+      </c>
       <c r="W15" s="8" t="n">
         <v>43264</v>
       </c>
       <c r="X15" s="8" t="n"/>
       <c r="Y15" s="8" t="n"/>
-      <c r="Z15" s="8" t="n">
+      <c r="Z15" s="8" t="n"/>
+      <c r="AA15" s="8" t="n">
         <v>43264</v>
       </c>
     </row>
@@ -1515,55 +1603,62 @@
       </c>
       <c r="D16" s="8" t="n"/>
       <c r="E16" s="8" t="n"/>
-      <c r="F16" s="8" t="n">
+      <c r="F16" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-12</t>
+        </is>
+      </c>
+      <c r="G16" s="8" t="n"/>
+      <c r="H16" s="8" t="inlineStr">
+        <is>
+          <t>AdaptiveAvgPool2d: 1-2</t>
+        </is>
+      </c>
+      <c r="I16" s="8" t="n"/>
+      <c r="J16" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="G16" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="H16" s="8" t="n">
-        <v>13</v>
-      </c>
-      <c r="I16" s="8" t="n">
+      <c r="K16" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="L16" s="8" t="n">
+        <v>13</v>
+      </c>
+      <c r="M16" s="8" t="n">
         <v>256</v>
       </c>
-      <c r="J16" s="8" t="n">
+      <c r="N16" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="K16" s="8" t="n">
+      <c r="O16" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="L16" s="8" t="n">
+      <c r="P16" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="M16" s="8" t="n">
+      <c r="Q16" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="N16" s="8" t="n">
+      <c r="R16" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="O16" s="8" t="n"/>
-      <c r="P16" s="8" t="n">
+      <c r="S16" s="8" t="n"/>
+      <c r="T16" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="Q16" s="8" t="n"/>
-      <c r="R16" s="8" t="n">
-        <v>43264</v>
-      </c>
-      <c r="S16" s="8" t="n">
-        <v>9216</v>
-      </c>
-      <c r="T16" s="8" t="n"/>
       <c r="U16" s="8" t="n"/>
       <c r="V16" s="8" t="n">
+        <v>43264</v>
+      </c>
+      <c r="W16" s="8" t="n">
+        <v>9216</v>
+      </c>
+      <c r="X16" s="8" t="n"/>
+      <c r="Y16" s="8" t="n"/>
+      <c r="Z16" s="8" t="n">
         <v>73728</v>
       </c>
-      <c r="W16" s="8" t="n"/>
-      <c r="X16" s="8" t="n"/>
-      <c r="Y16" s="8" t="n">
-        <v>1557504</v>
-      </c>
-      <c r="Z16" s="8" t="n"/>
+      <c r="AA16" s="8" t="n"/>
     </row>
     <row r="17">
       <c r="A17" s="7" t="n">
@@ -1577,43 +1672,52 @@
       <c r="C17" s="8" t="n"/>
       <c r="D17" s="8" t="n"/>
       <c r="E17" s="8" t="n"/>
-      <c r="F17" s="8" t="n">
+      <c r="F17" s="8" t="inlineStr">
+        <is>
+          <t>MaxPool2d: 2-13</t>
+        </is>
+      </c>
+      <c r="G17" s="8" t="n"/>
+      <c r="H17" s="8" t="inlineStr">
+        <is>
+          <t>Dropout: 2-14</t>
+        </is>
+      </c>
+      <c r="I17" s="8" t="n"/>
+      <c r="J17" s="8" t="n">
         <v>256</v>
-      </c>
-      <c r="G17" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="H17" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="I17" s="8" t="n">
-        <v>256</v>
-      </c>
-      <c r="J17" s="8" t="n">
-        <v>6</v>
       </c>
       <c r="K17" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="L17" s="8" t="n"/>
-      <c r="M17" s="8" t="n"/>
-      <c r="N17" s="8" t="n"/>
-      <c r="O17" s="8" t="n"/>
+      <c r="L17" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="M17" s="8" t="n">
+        <v>256</v>
+      </c>
+      <c r="N17" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="O17" s="8" t="n">
+        <v>6</v>
+      </c>
       <c r="P17" s="8" t="n"/>
       <c r="Q17" s="8" t="n"/>
-      <c r="R17" s="8" t="n">
-        <v>9216</v>
-      </c>
-      <c r="S17" s="8" t="n">
-        <v>9216</v>
-      </c>
+      <c r="R17" s="8" t="n"/>
+      <c r="S17" s="8" t="n"/>
       <c r="T17" s="8" t="n"/>
       <c r="U17" s="8" t="n"/>
-      <c r="V17" s="8" t="n"/>
-      <c r="W17" s="8" t="n"/>
+      <c r="V17" s="8" t="n">
+        <v>9216</v>
+      </c>
+      <c r="W17" s="8" t="n">
+        <v>9216</v>
+      </c>
       <c r="X17" s="8" t="n"/>
       <c r="Y17" s="8" t="n"/>
       <c r="Z17" s="8" t="n"/>
+      <c r="AA17" s="8" t="n"/>
     </row>
     <row r="18">
       <c r="A18" s="7" t="n">
@@ -1627,43 +1731,48 @@
       <c r="C18" s="8" t="n"/>
       <c r="D18" s="8" t="n"/>
       <c r="E18" s="8" t="n"/>
-      <c r="F18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" s="8" t="n">
-        <v>0</v>
-      </c>
+      <c r="F18" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-19</t>
+        </is>
+      </c>
+      <c r="G18" s="8" t="n"/>
+      <c r="H18" s="8" t="n"/>
+      <c r="I18" s="8" t="n"/>
       <c r="J18" s="8" t="n">
         <v>0</v>
       </c>
       <c r="K18" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="L18" s="8" t="n"/>
-      <c r="M18" s="8" t="n"/>
-      <c r="N18" s="8" t="n"/>
-      <c r="O18" s="8" t="n"/>
+      <c r="L18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" s="8" t="n">
+        <v>0</v>
+      </c>
       <c r="P18" s="8" t="n"/>
       <c r="Q18" s="8" t="n"/>
-      <c r="R18" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S18" s="8" t="n">
-        <v>0</v>
-      </c>
+      <c r="R18" s="8" t="n"/>
+      <c r="S18" s="8" t="n"/>
       <c r="T18" s="8" t="n"/>
       <c r="U18" s="8" t="n"/>
-      <c r="V18" s="8" t="n"/>
-      <c r="W18" s="8" t="n"/>
+      <c r="V18" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="W18" s="8" t="n">
+        <v>0</v>
+      </c>
       <c r="X18" s="8" t="n"/>
       <c r="Y18" s="8" t="n"/>
       <c r="Z18" s="8" t="n"/>
+      <c r="AA18" s="8" t="n"/>
     </row>
     <row r="19">
       <c r="A19" s="7" t="n">
@@ -1677,35 +1786,44 @@
       </c>
       <c r="D19" s="8" t="n"/>
       <c r="E19" s="8" t="n"/>
-      <c r="F19" s="8" t="n">
+      <c r="F19" s="8" t="inlineStr">
+        <is>
+          <t>AdaptiveAvgPool2d: 1-2</t>
+        </is>
+      </c>
+      <c r="G19" s="8" t="n"/>
+      <c r="H19" s="8" t="inlineStr">
+        <is>
+          <t>Linear: 2-15</t>
+        </is>
+      </c>
+      <c r="I19" s="8" t="n"/>
+      <c r="J19" s="8" t="n">
         <v>9216</v>
       </c>
-      <c r="G19" s="8" t="n"/>
-      <c r="H19" s="8" t="n"/>
-      <c r="I19" s="8" t="n">
-        <v>9216</v>
-      </c>
-      <c r="J19" s="8" t="n"/>
       <c r="K19" s="8" t="n"/>
       <c r="L19" s="8" t="n"/>
-      <c r="M19" s="8" t="n"/>
+      <c r="M19" s="8" t="n">
+        <v>9216</v>
+      </c>
       <c r="N19" s="8" t="n"/>
       <c r="O19" s="8" t="n"/>
       <c r="P19" s="8" t="n"/>
       <c r="Q19" s="8" t="n"/>
-      <c r="R19" s="8" t="n">
-        <v>9216</v>
-      </c>
-      <c r="S19" s="8" t="n">
-        <v>9216</v>
-      </c>
+      <c r="R19" s="8" t="n"/>
+      <c r="S19" s="8" t="n"/>
       <c r="T19" s="8" t="n"/>
       <c r="U19" s="8" t="n"/>
-      <c r="V19" s="8" t="n"/>
-      <c r="W19" s="8" t="n"/>
+      <c r="V19" s="8" t="n">
+        <v>9216</v>
+      </c>
+      <c r="W19" s="8" t="n">
+        <v>9216</v>
+      </c>
       <c r="X19" s="8" t="n"/>
       <c r="Y19" s="8" t="n"/>
       <c r="Z19" s="8" t="n"/>
+      <c r="AA19" s="8" t="n"/>
     </row>
     <row r="20">
       <c r="A20" s="7" t="n">
@@ -1719,41 +1837,48 @@
       </c>
       <c r="D20" s="8" t="n"/>
       <c r="E20" s="8" t="n"/>
-      <c r="F20" s="8" t="n">
+      <c r="F20" s="8" t="inlineStr">
+        <is>
+          <t>Dropout: 2-14</t>
+        </is>
+      </c>
+      <c r="G20" s="8" t="n"/>
+      <c r="H20" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-16</t>
+        </is>
+      </c>
+      <c r="I20" s="8" t="n"/>
+      <c r="J20" s="8" t="n">
         <v>9216</v>
       </c>
-      <c r="G20" s="8" t="n"/>
-      <c r="H20" s="8" t="n"/>
-      <c r="I20" s="8" t="n">
-        <v>4096</v>
-      </c>
-      <c r="J20" s="8" t="n"/>
       <c r="K20" s="8" t="n"/>
       <c r="L20" s="8" t="n"/>
-      <c r="M20" s="8" t="n"/>
+      <c r="M20" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="N20" s="8" t="n"/>
       <c r="O20" s="8" t="n"/>
       <c r="P20" s="8" t="n"/>
       <c r="Q20" s="8" t="n"/>
-      <c r="R20" s="8" t="n">
+      <c r="R20" s="8" t="n"/>
+      <c r="S20" s="8" t="n"/>
+      <c r="T20" s="8" t="n"/>
+      <c r="U20" s="8" t="n"/>
+      <c r="V20" s="8" t="n">
         <v>9216</v>
       </c>
-      <c r="S20" s="8" t="n">
+      <c r="W20" s="8" t="n">
         <v>4096</v>
       </c>
-      <c r="T20" s="8" t="n">
+      <c r="X20" s="8" t="n">
         <v>37752832</v>
       </c>
-      <c r="U20" s="8" t="n">
+      <c r="Y20" s="8" t="n">
         <v>37748736</v>
       </c>
-      <c r="V20" s="8" t="n"/>
-      <c r="W20" s="8" t="n"/>
-      <c r="X20" s="8" t="n">
-        <v>37748736</v>
-      </c>
-      <c r="Y20" s="8" t="n"/>
       <c r="Z20" s="8" t="n"/>
+      <c r="AA20" s="8" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="7" t="n">
@@ -1762,42 +1887,49 @@
       <c r="B21" s="8" t="n"/>
       <c r="C21" s="8" t="inlineStr">
         <is>
-          <t>ReLU: 2-16</t>
+          <t>ReLU(inplace): 2-16</t>
         </is>
       </c>
       <c r="D21" s="8" t="n"/>
       <c r="E21" s="8" t="n"/>
-      <c r="F21" s="8" t="n">
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>Linear: 2-15</t>
+        </is>
+      </c>
+      <c r="G21" s="8" t="n"/>
+      <c r="H21" s="8" t="inlineStr">
+        <is>
+          <t>Dropout: 2-17</t>
+        </is>
+      </c>
+      <c r="I21" s="8" t="n"/>
+      <c r="J21" s="8" t="n">
         <v>4096</v>
       </c>
-      <c r="G21" s="8" t="n"/>
-      <c r="H21" s="8" t="n"/>
-      <c r="I21" s="8" t="n">
-        <v>4096</v>
-      </c>
-      <c r="J21" s="8" t="n"/>
       <c r="K21" s="8" t="n"/>
       <c r="L21" s="8" t="n"/>
-      <c r="M21" s="8" t="n"/>
+      <c r="M21" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="N21" s="8" t="n"/>
       <c r="O21" s="8" t="n"/>
       <c r="P21" s="8" t="n"/>
       <c r="Q21" s="8" t="n"/>
-      <c r="R21" s="8" t="n">
-        <v>4096</v>
-      </c>
-      <c r="S21" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="R21" s="8" t="n"/>
+      <c r="S21" s="8" t="n"/>
       <c r="T21" s="8" t="n"/>
       <c r="U21" s="8" t="n"/>
-      <c r="V21" s="8" t="n"/>
+      <c r="V21" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="W21" s="8" t="n">
         <v>4096</v>
       </c>
       <c r="X21" s="8" t="n"/>
       <c r="Y21" s="8" t="n"/>
-      <c r="Z21" s="8" t="n">
+      <c r="Z21" s="8" t="n"/>
+      <c r="AA21" s="8" t="n">
         <v>4096</v>
       </c>
     </row>
@@ -1813,35 +1945,44 @@
       </c>
       <c r="D22" s="8" t="n"/>
       <c r="E22" s="8" t="n"/>
-      <c r="F22" s="8" t="n">
+      <c r="F22" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-16</t>
+        </is>
+      </c>
+      <c r="G22" s="8" t="n"/>
+      <c r="H22" s="8" t="inlineStr">
+        <is>
+          <t>Linear: 2-18</t>
+        </is>
+      </c>
+      <c r="I22" s="8" t="n"/>
+      <c r="J22" s="8" t="n">
         <v>4096</v>
       </c>
-      <c r="G22" s="8" t="n"/>
-      <c r="H22" s="8" t="n"/>
-      <c r="I22" s="8" t="n">
-        <v>4096</v>
-      </c>
-      <c r="J22" s="8" t="n"/>
       <c r="K22" s="8" t="n"/>
       <c r="L22" s="8" t="n"/>
-      <c r="M22" s="8" t="n"/>
+      <c r="M22" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="N22" s="8" t="n"/>
       <c r="O22" s="8" t="n"/>
       <c r="P22" s="8" t="n"/>
       <c r="Q22" s="8" t="n"/>
-      <c r="R22" s="8" t="n">
-        <v>4096</v>
-      </c>
-      <c r="S22" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="R22" s="8" t="n"/>
+      <c r="S22" s="8" t="n"/>
       <c r="T22" s="8" t="n"/>
       <c r="U22" s="8" t="n"/>
-      <c r="V22" s="8" t="n"/>
-      <c r="W22" s="8" t="n"/>
+      <c r="V22" s="8" t="n">
+        <v>4096</v>
+      </c>
+      <c r="W22" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="X22" s="8" t="n"/>
       <c r="Y22" s="8" t="n"/>
       <c r="Z22" s="8" t="n"/>
+      <c r="AA22" s="8" t="n"/>
     </row>
     <row r="23">
       <c r="A23" s="7" t="n">
@@ -1855,41 +1996,48 @@
       </c>
       <c r="D23" s="8" t="n"/>
       <c r="E23" s="8" t="n"/>
-      <c r="F23" s="8" t="n">
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>Dropout: 2-17</t>
+        </is>
+      </c>
+      <c r="G23" s="8" t="n"/>
+      <c r="H23" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-19</t>
+        </is>
+      </c>
+      <c r="I23" s="8" t="n"/>
+      <c r="J23" s="8" t="n">
         <v>4096</v>
       </c>
-      <c r="G23" s="8" t="n"/>
-      <c r="H23" s="8" t="n"/>
-      <c r="I23" s="8" t="n">
-        <v>4096</v>
-      </c>
-      <c r="J23" s="8" t="n"/>
       <c r="K23" s="8" t="n"/>
       <c r="L23" s="8" t="n"/>
-      <c r="M23" s="8" t="n"/>
+      <c r="M23" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="N23" s="8" t="n"/>
       <c r="O23" s="8" t="n"/>
       <c r="P23" s="8" t="n"/>
       <c r="Q23" s="8" t="n"/>
-      <c r="R23" s="8" t="n">
+      <c r="R23" s="8" t="n"/>
+      <c r="S23" s="8" t="n"/>
+      <c r="T23" s="8" t="n"/>
+      <c r="U23" s="8" t="n"/>
+      <c r="V23" s="8" t="n">
         <v>4096</v>
       </c>
-      <c r="S23" s="8" t="n">
+      <c r="W23" s="8" t="n">
         <v>4096</v>
       </c>
-      <c r="T23" s="8" t="n">
+      <c r="X23" s="8" t="n">
         <v>16781312</v>
       </c>
-      <c r="U23" s="8" t="n">
+      <c r="Y23" s="8" t="n">
         <v>16777216</v>
       </c>
-      <c r="V23" s="8" t="n"/>
-      <c r="W23" s="8" t="n"/>
-      <c r="X23" s="8" t="n">
-        <v>16777216</v>
-      </c>
-      <c r="Y23" s="8" t="n"/>
       <c r="Z23" s="8" t="n"/>
+      <c r="AA23" s="8" t="n"/>
     </row>
     <row r="24">
       <c r="A24" s="7" t="n">
@@ -1898,42 +2046,49 @@
       <c r="B24" s="8" t="n"/>
       <c r="C24" s="8" t="inlineStr">
         <is>
-          <t>ReLU: 2-19</t>
+          <t>ReLU(inplace): 2-19</t>
         </is>
       </c>
       <c r="D24" s="8" t="n"/>
       <c r="E24" s="8" t="n"/>
-      <c r="F24" s="8" t="n">
+      <c r="F24" s="8" t="inlineStr">
+        <is>
+          <t>Linear: 2-18</t>
+        </is>
+      </c>
+      <c r="G24" s="8" t="n"/>
+      <c r="H24" s="8" t="inlineStr">
+        <is>
+          <t>Linear: 2-20</t>
+        </is>
+      </c>
+      <c r="I24" s="8" t="n"/>
+      <c r="J24" s="8" t="n">
         <v>4096</v>
       </c>
-      <c r="G24" s="8" t="n"/>
-      <c r="H24" s="8" t="n"/>
-      <c r="I24" s="8" t="n">
-        <v>4096</v>
-      </c>
-      <c r="J24" s="8" t="n"/>
       <c r="K24" s="8" t="n"/>
       <c r="L24" s="8" t="n"/>
-      <c r="M24" s="8" t="n"/>
+      <c r="M24" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="N24" s="8" t="n"/>
       <c r="O24" s="8" t="n"/>
       <c r="P24" s="8" t="n"/>
       <c r="Q24" s="8" t="n"/>
-      <c r="R24" s="8" t="n">
-        <v>4096</v>
-      </c>
-      <c r="S24" s="8" t="n">
-        <v>4096</v>
-      </c>
+      <c r="R24" s="8" t="n"/>
+      <c r="S24" s="8" t="n"/>
       <c r="T24" s="8" t="n"/>
       <c r="U24" s="8" t="n"/>
-      <c r="V24" s="8" t="n"/>
+      <c r="V24" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="W24" s="8" t="n">
         <v>4096</v>
       </c>
       <c r="X24" s="8" t="n"/>
       <c r="Y24" s="8" t="n"/>
-      <c r="Z24" s="8" t="n">
+      <c r="Z24" s="8" t="n"/>
+      <c r="AA24" s="8" t="n">
         <v>4096</v>
       </c>
     </row>
@@ -1949,72 +2104,70 @@
       </c>
       <c r="D25" s="8" t="n"/>
       <c r="E25" s="8" t="n"/>
-      <c r="F25" s="8" t="n">
-        <v>4096</v>
+      <c r="F25" s="8" t="inlineStr">
+        <is>
+          <t>ReLU(inplace): 2-19</t>
+        </is>
       </c>
       <c r="G25" s="8" t="n"/>
       <c r="H25" s="8" t="n"/>
-      <c r="I25" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="J25" s="8" t="n"/>
+      <c r="I25" s="8" t="n"/>
+      <c r="J25" s="8" t="n">
+        <v>4096</v>
+      </c>
       <c r="K25" s="8" t="n"/>
       <c r="L25" s="8" t="n"/>
-      <c r="M25" s="8" t="n"/>
+      <c r="M25" s="8" t="n">
+        <v>1000</v>
+      </c>
       <c r="N25" s="8" t="n"/>
       <c r="O25" s="8" t="n"/>
       <c r="P25" s="8" t="n"/>
       <c r="Q25" s="8" t="n"/>
-      <c r="R25" s="8" t="n">
+      <c r="R25" s="8" t="n"/>
+      <c r="S25" s="8" t="n"/>
+      <c r="T25" s="8" t="n"/>
+      <c r="U25" s="8" t="n"/>
+      <c r="V25" s="8" t="n">
         <v>4096</v>
       </c>
-      <c r="S25" s="8" t="n">
+      <c r="W25" s="8" t="n">
         <v>1000</v>
       </c>
-      <c r="T25" s="8" t="n">
+      <c r="X25" s="8" t="n">
         <v>4097000</v>
       </c>
-      <c r="U25" s="8" t="n">
+      <c r="Y25" s="8" t="n">
         <v>4096000</v>
       </c>
-      <c r="V25" s="8" t="n"/>
-      <c r="W25" s="8" t="n"/>
-      <c r="X25" s="8" t="n">
-        <v>4096000</v>
-      </c>
-      <c r="Y25" s="8" t="n"/>
       <c r="Z25" s="8" t="n"/>
+      <c r="AA25" s="8" t="n"/>
     </row>
   </sheetData>
   <mergeCells count="9">
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="M1:O1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:T1"/>
-    <mergeCell ref="U1:W1"/>
-    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
   </mergeCells>
-  <conditionalFormatting sqref="S1:S25">
+  <conditionalFormatting sqref="W1:W25">
     <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
       <formula>193600</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="T1:T25">
+  <conditionalFormatting sqref="X1:X25">
     <cfRule type="cellIs" priority="2" operator="equal" dxfId="1" stopIfTrue="1">
       <formula>37752832</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U1:U25">
+  <conditionalFormatting sqref="Y1:Y25">
     <cfRule type="cellIs" priority="3" operator="equal" dxfId="2" stopIfTrue="1">
       <formula>224088768</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X1:X25">
-    <cfRule type="cellIs" priority="4" operator="equal" dxfId="3" stopIfTrue="1">
-      <formula>1165688832</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2027,7 +2180,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2076,16 +2229,6 @@
         <v>0.714673472</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="8" t="inlineStr">
-        <is>
-          <t>Total Backward GEMM (G_ops):</t>
-        </is>
-      </c>
-      <c r="B5" s="8" t="n">
-        <v>1.809600512</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>